<commit_message>
Revisão geral do código.
</commit_message>
<xml_diff>
--- a/Auxiliares/Atlas_Desenvolvimento_Humano_Brasil_2010/AtlasBrasil_Consulta.xlsx
+++ b/Auxiliares/Atlas_Desenvolvimento_Humano_Brasil_2010/AtlasBrasil_Consulta.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="188">
   <si>
     <t>Código</t>
   </si>
@@ -24,9 +24,6 @@
   </si>
   <si>
     <t>IDHM 2010</t>
-  </si>
-  <si>
-    <t>Desagregação Mulher IDHM 2010</t>
   </si>
   <si>
     <t>Brasil</t>
@@ -920,7 +917,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D186"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -928,7 +925,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -938,2052 +935,2037 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2">
         <v>0.727</v>
       </c>
-      <c r="D2">
-        <v>0.756</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2300101</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0.628</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>2300150</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>0.606</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>2300200</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>0.601</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2300309</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>0.595</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>2300408</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>0.569</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>2300507</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>2300606</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9">
         <v>0.602</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>2300705</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>0.601</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>2300754</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11">
         <v>0.606</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2300804</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12">
         <v>0.599</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>2300903</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>0.618</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>2301000</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>0.641</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>2301109</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15">
         <v>0.655</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>2301208</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16">
         <v>0.615</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>2301257</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17">
         <v>0.59</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>2301307</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C18">
         <v>0.5639999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>2301406</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19">
         <v>0.622</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>2301505</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20">
         <v>0.618</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>2301604</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21">
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>2301703</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22">
         <v>0.605</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:3">
       <c r="A23">
         <v>2301802</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23">
         <v>0.627</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:3">
       <c r="A24">
         <v>2301851</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24">
         <v>0.606</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:3">
       <c r="A25">
         <v>2301901</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25">
         <v>0.6830000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:3">
       <c r="A26">
         <v>2301950</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26">
         <v>0.616</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>2302008</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27">
         <v>0.599</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>2302057</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28">
         <v>0.571</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>2302107</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29">
         <v>0.619</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>2302206</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30">
         <v>0.638</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>2302305</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31">
         <v>0.623</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>2302404</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32">
         <v>0.598</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:3">
       <c r="A33">
         <v>2302503</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33">
         <v>0.647</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:3">
       <c r="A34">
         <v>2302602</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34">
         <v>0.62</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>2302701</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35">
         <v>0.63</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>2302800</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36">
         <v>0.612</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>2302909</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37">
         <v>0.611</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>2303006</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38">
         <v>0.592</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>2303105</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>0.596</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>2303204</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C40">
         <v>0.578</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>2303303</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41">
         <v>0.597</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>2303402</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C42">
         <v>0.593</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>2303501</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C43">
         <v>0.646</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>2303600</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44">
         <v>0.618</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:3">
       <c r="A45">
         <v>2303659</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C45">
         <v>0.609</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:3">
       <c r="A46">
         <v>2303709</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46">
         <v>0.6820000000000001</v>
       </c>
-      <c r="D46">
-        <v>0.707</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+    </row>
+    <row r="47" spans="1:3">
       <c r="A47">
         <v>2303808</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47">
         <v>0.627</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:3">
       <c r="A48">
         <v>2303907</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48">
         <v>0.586</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:3">
       <c r="A49">
         <v>2303931</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C49">
         <v>0.585</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:3">
       <c r="A50">
         <v>2303956</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C50">
         <v>0.604</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:3">
       <c r="A51">
         <v>2304004</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C51">
         <v>0.61</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:3">
       <c r="A52">
         <v>2304103</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52">
         <v>0.644</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:3">
       <c r="A53">
         <v>2304202</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53">
         <v>0.713</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:3">
       <c r="A54">
         <v>2304236</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C54">
         <v>0.59</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:3">
       <c r="A55">
         <v>2304251</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C55">
         <v>0.632</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:3">
       <c r="A56">
         <v>2304269</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C56">
         <v>0.609</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:3">
       <c r="A57">
         <v>2304277</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C57">
         <v>0.61</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:3">
       <c r="A58">
         <v>2304285</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C58">
         <v>0.701</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:3">
       <c r="A59">
         <v>2304301</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C59">
         <v>0.633</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:3">
       <c r="A60">
         <v>2304350</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C60">
         <v>0.644</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:3">
       <c r="A61">
         <v>2304400</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C61">
         <v>0.754</v>
       </c>
-      <c r="D61">
-        <v>0.783</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62">
         <v>2304459</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C62">
         <v>0.624</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:3">
       <c r="A63">
         <v>2304509</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63">
         <v>0.604</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:3">
       <c r="A64">
         <v>2304608</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C64">
         <v>0.5679999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:3">
       <c r="A65">
         <v>2304657</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C65">
         <v>0.57</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:3">
       <c r="A66">
         <v>2304707</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C66">
         <v>0.5590000000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:3">
       <c r="A67">
         <v>2304806</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C67">
         <v>0.585</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:3">
       <c r="A68">
         <v>2304905</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C68">
         <v>0.633</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:3">
       <c r="A69">
         <v>2304954</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C69">
         <v>0.617</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:3">
       <c r="A70">
         <v>2305001</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C70">
         <v>0.609</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:3">
       <c r="A71">
         <v>2305100</v>
       </c>
       <c r="B71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C71">
         <v>0.637</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:3">
       <c r="A72">
         <v>2305209</v>
       </c>
       <c r="B72" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C72">
         <v>0.597</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:3">
       <c r="A73">
         <v>2305233</v>
       </c>
       <c r="B73" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C73">
         <v>0.658</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:3">
       <c r="A74">
         <v>2305266</v>
       </c>
       <c r="B74" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C74">
         <v>0.577</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:3">
       <c r="A75">
         <v>2305308</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C75">
         <v>0.608</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:3">
       <c r="A76">
         <v>2305332</v>
       </c>
       <c r="B76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C76">
         <v>0.606</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:3">
       <c r="A77">
         <v>2305357</v>
       </c>
       <c r="B77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C77">
         <v>0.616</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:3">
       <c r="A78">
         <v>2305407</v>
       </c>
       <c r="B78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C78">
         <v>0.606</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:3">
       <c r="A79">
         <v>2305506</v>
       </c>
       <c r="B79" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C79">
         <v>0.677</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:3">
       <c r="A80">
         <v>2305605</v>
       </c>
       <c r="B80" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C80">
         <v>0.632</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:3">
       <c r="A81">
         <v>2305654</v>
       </c>
       <c r="B81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C81">
         <v>0.579</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:3">
       <c r="A82">
         <v>2305704</v>
       </c>
       <c r="B82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C82">
         <v>0.606</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:3">
       <c r="A83">
         <v>2305803</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C83">
         <v>0.618</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:3">
       <c r="A84">
         <v>2305902</v>
       </c>
       <c r="B84" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C84">
         <v>0.573</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:3">
       <c r="A85">
         <v>2306009</v>
       </c>
       <c r="B85" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C85">
         <v>0.652</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:3">
       <c r="A86">
         <v>2306108</v>
       </c>
       <c r="B86" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C86">
         <v>0.605</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:3">
       <c r="A87">
         <v>2306207</v>
       </c>
       <c r="B87" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C87">
         <v>0.656</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:3">
       <c r="A88">
         <v>2306256</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C88">
         <v>0.626</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:3">
       <c r="A89">
         <v>2306306</v>
       </c>
       <c r="B89" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C89">
         <v>0.623</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:3">
       <c r="A90">
         <v>2306405</v>
       </c>
       <c r="B90" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C90">
         <v>0.64</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:3">
       <c r="A91">
         <v>2306504</v>
       </c>
       <c r="B91" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C91">
         <v>0.604</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:3">
       <c r="A92">
         <v>2306553</v>
       </c>
       <c r="B92" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C92">
         <v>0.606</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:3">
       <c r="A93">
         <v>2306603</v>
       </c>
       <c r="B93" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C93">
         <v>0.5620000000000001</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:3">
       <c r="A94">
         <v>2306702</v>
       </c>
       <c r="B94" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C94">
         <v>0.612</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:3">
       <c r="A95">
         <v>2306801</v>
       </c>
       <c r="B95" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C95">
         <v>0.618</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:3">
       <c r="A96">
         <v>2306900</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C96">
         <v>0.621</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:3">
       <c r="A97">
         <v>2307007</v>
       </c>
       <c r="B97" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C97">
         <v>0.624</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:3">
       <c r="A98">
         <v>2307106</v>
       </c>
       <c r="B98" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C98">
         <v>0.614</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:3">
       <c r="A99">
         <v>2307205</v>
       </c>
       <c r="B99" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C99">
         <v>0.651</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:3">
       <c r="A100">
         <v>2307254</v>
       </c>
       <c r="B100" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C100">
         <v>0.652</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:3">
       <c r="A101">
         <v>2307304</v>
       </c>
       <c r="B101" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C101">
         <v>0.694</v>
       </c>
-      <c r="D101">
-        <v>0.727</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4">
+    </row>
+    <row r="102" spans="1:3">
       <c r="A102">
         <v>2307403</v>
       </c>
       <c r="B102" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C102">
         <v>0.598</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:3">
       <c r="A103">
         <v>2307502</v>
       </c>
       <c r="B103" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C103">
         <v>0.613</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:3">
       <c r="A104">
         <v>2307601</v>
       </c>
       <c r="B104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C104">
         <v>0.6820000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:3">
       <c r="A105">
         <v>2307635</v>
       </c>
       <c r="B105" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C105">
         <v>0.61</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:3">
       <c r="A106">
         <v>2307650</v>
       </c>
       <c r="B106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C106">
         <v>0.6860000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:3">
       <c r="A107">
         <v>2307700</v>
       </c>
       <c r="B107" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C107">
         <v>0.659</v>
       </c>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:3">
       <c r="A108">
         <v>2307809</v>
       </c>
       <c r="B108" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C108">
         <v>0.612</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:3">
       <c r="A109">
         <v>2307908</v>
       </c>
       <c r="B109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C109">
         <v>0.599</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:3">
       <c r="A110">
         <v>2308005</v>
       </c>
       <c r="B110" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C110">
         <v>0.616</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:3">
       <c r="A111">
         <v>2308104</v>
       </c>
       <c r="B111" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C111">
         <v>0.605</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:3">
       <c r="A112">
         <v>2308203</v>
       </c>
       <c r="B112" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C112">
         <v>0.618</v>
       </c>
     </row>
-    <row r="113" spans="1:4">
+    <row r="113" spans="1:3">
       <c r="A113">
         <v>2308302</v>
       </c>
       <c r="B113" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C113">
         <v>0.628</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:3">
       <c r="A114">
         <v>2308351</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C114">
         <v>0.626</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:3">
       <c r="A115">
         <v>2308377</v>
       </c>
       <c r="B115" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C115">
         <v>0.592</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:3">
       <c r="A116">
         <v>2308401</v>
       </c>
       <c r="B116" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C116">
         <v>0.622</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:3">
       <c r="A117">
         <v>2308500</v>
       </c>
       <c r="B117" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C117">
         <v>0.582</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:3">
       <c r="A118">
         <v>2308609</v>
       </c>
       <c r="B118" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C118">
         <v>0.61</v>
       </c>
     </row>
-    <row r="119" spans="1:4">
+    <row r="119" spans="1:3">
       <c r="A119">
         <v>2308708</v>
       </c>
       <c r="B119" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C119">
         <v>0.61</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:3">
       <c r="A120">
         <v>2308807</v>
       </c>
       <c r="B120" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C120">
         <v>0.581</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:3">
       <c r="A121">
         <v>2308906</v>
       </c>
       <c r="B121" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C121">
         <v>0.588</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:3">
       <c r="A122">
         <v>2309003</v>
       </c>
       <c r="B122" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C122">
         <v>0.607</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:3">
       <c r="A123">
         <v>2309102</v>
       </c>
       <c r="B123" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C123">
         <v>0.607</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:3">
       <c r="A124">
         <v>2309201</v>
       </c>
       <c r="B124" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C124">
         <v>0.625</v>
       </c>
     </row>
-    <row r="125" spans="1:4">
+    <row r="125" spans="1:3">
       <c r="A125">
         <v>2309300</v>
       </c>
       <c r="B125" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C125">
         <v>0.614</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:3">
       <c r="A126">
         <v>2309409</v>
       </c>
       <c r="B126" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C126">
         <v>0.605</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:3">
       <c r="A127">
         <v>2309458</v>
       </c>
       <c r="B127" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C127">
         <v>0.594</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:3">
       <c r="A128">
         <v>2309508</v>
       </c>
       <c r="B128" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C128">
         <v>0.636</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:3">
       <c r="A129">
         <v>2309607</v>
       </c>
       <c r="B129" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C129">
         <v>0.659</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:3">
       <c r="A130">
         <v>2309706</v>
       </c>
       <c r="B130" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C130">
         <v>0.675</v>
       </c>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:3">
       <c r="A131">
         <v>2309805</v>
       </c>
       <c r="B131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C131">
         <v>0.635</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:3">
       <c r="A132">
         <v>2309904</v>
       </c>
       <c r="B132" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C132">
         <v>0.621</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:3">
       <c r="A133">
         <v>2310001</v>
       </c>
       <c r="B133" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C133">
         <v>0.638</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:3">
       <c r="A134">
         <v>2310100</v>
       </c>
       <c r="B134" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C134">
         <v>0.622</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:3">
       <c r="A135">
         <v>2310209</v>
       </c>
       <c r="B135" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C135">
         <v>0.637</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:3">
       <c r="A136">
         <v>2310258</v>
       </c>
       <c r="B136" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C136">
         <v>0.634</v>
       </c>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:3">
       <c r="A137">
         <v>2310308</v>
       </c>
       <c r="B137" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C137">
         <v>0.57</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:3">
       <c r="A138">
         <v>2310407</v>
       </c>
       <c r="B138" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C138">
         <v>0.583</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:3">
       <c r="A139">
         <v>2310506</v>
       </c>
       <c r="B139" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C139">
         <v>0.603</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:3">
       <c r="A140">
         <v>2310605</v>
       </c>
       <c r="B140" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C140">
         <v>0.646</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:3">
       <c r="A141">
         <v>2310704</v>
       </c>
       <c r="B141" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C141">
         <v>0.629</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:3">
       <c r="A142">
         <v>2310803</v>
       </c>
       <c r="B142" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C142">
         <v>0.601</v>
       </c>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:3">
       <c r="A143">
         <v>2310852</v>
       </c>
       <c r="B143" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C143">
         <v>0.636</v>
       </c>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:3">
       <c r="A144">
         <v>2310902</v>
       </c>
       <c r="B144" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C144">
         <v>0.6</v>
       </c>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:3">
       <c r="A145">
         <v>2310951</v>
       </c>
       <c r="B145" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C145">
         <v>0.591</v>
       </c>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:3">
       <c r="A146">
         <v>2311009</v>
       </c>
       <c r="B146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C146">
         <v>0.581</v>
       </c>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:3">
       <c r="A147">
         <v>2311108</v>
       </c>
       <c r="B147" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C147">
         <v>0.622</v>
       </c>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:3">
       <c r="A148">
         <v>2311207</v>
       </c>
       <c r="B148" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C148">
         <v>0.5620000000000001</v>
       </c>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:3">
       <c r="A149">
         <v>2311231</v>
       </c>
       <c r="B149" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C149">
         <v>0.604</v>
       </c>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:3">
       <c r="A150">
         <v>2311264</v>
       </c>
       <c r="B150" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C150">
         <v>0.594</v>
       </c>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:3">
       <c r="A151">
         <v>2311306</v>
       </c>
       <c r="B151" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C151">
         <v>0.659</v>
       </c>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:3">
       <c r="A152">
         <v>2311355</v>
       </c>
       <c r="B152" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C152">
         <v>0.591</v>
       </c>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:3">
       <c r="A153">
         <v>2311405</v>
       </c>
       <c r="B153" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C153">
         <v>0.642</v>
       </c>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:3">
       <c r="A154">
         <v>2311504</v>
       </c>
       <c r="B154" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C154">
         <v>0.622</v>
       </c>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:3">
       <c r="A155">
         <v>2311603</v>
       </c>
       <c r="B155" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C155">
         <v>0.626</v>
       </c>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:3">
       <c r="A156">
         <v>2311702</v>
       </c>
       <c r="B156" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C156">
         <v>0.601</v>
       </c>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:3">
       <c r="A157">
         <v>2311801</v>
       </c>
       <c r="B157" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C157">
         <v>0.674</v>
       </c>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:3">
       <c r="A158">
         <v>2311900</v>
       </c>
       <c r="B158" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C158">
         <v>0.575</v>
       </c>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:3">
       <c r="A159">
         <v>2311959</v>
       </c>
       <c r="B159" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C159">
         <v>0.54</v>
       </c>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:3">
       <c r="A160">
         <v>2312007</v>
       </c>
       <c r="B160" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C160">
         <v>0.587</v>
       </c>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:3">
       <c r="A161">
         <v>2312106</v>
       </c>
       <c r="B161" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C161">
         <v>0.612</v>
       </c>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:3">
       <c r="A162">
         <v>2312205</v>
       </c>
       <c r="B162" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C162">
         <v>0.616</v>
       </c>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:3">
       <c r="A163">
         <v>2312304</v>
       </c>
       <c r="B163" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C163">
         <v>0.611</v>
       </c>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:3">
       <c r="A164">
         <v>2312403</v>
       </c>
       <c r="B164" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C164">
         <v>0.665</v>
       </c>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:3">
       <c r="A165">
         <v>2312502</v>
       </c>
       <c r="B165" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C165">
         <v>0.654</v>
       </c>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:3">
       <c r="A166">
         <v>2312601</v>
       </c>
       <c r="B166" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C166">
         <v>0.62</v>
       </c>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:3">
       <c r="A167">
         <v>2312700</v>
       </c>
       <c r="B167" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C167">
         <v>0.619</v>
       </c>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:3">
       <c r="A168">
         <v>2312809</v>
       </c>
       <c r="B168" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C168">
         <v>0.603</v>
       </c>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:3">
       <c r="A169">
         <v>2312908</v>
       </c>
       <c r="B169" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C169">
         <v>0.714</v>
       </c>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:3">
       <c r="A170">
         <v>2313005</v>
       </c>
       <c r="B170" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C170">
         <v>0.625</v>
       </c>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:3">
       <c r="A171">
         <v>2313104</v>
       </c>
       <c r="B171" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C171">
         <v>0.645</v>
       </c>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:3">
       <c r="A172">
         <v>2313203</v>
       </c>
       <c r="B172" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C172">
         <v>0.58</v>
       </c>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:3">
       <c r="A173">
         <v>2313252</v>
       </c>
       <c r="B173" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C173">
         <v>0.576</v>
       </c>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:3">
       <c r="A174">
         <v>2313302</v>
       </c>
       <c r="B174" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C174">
         <v>0.633</v>
       </c>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:3">
       <c r="A175">
         <v>2313351</v>
       </c>
       <c r="B175" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C175">
         <v>0.584</v>
       </c>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:3">
       <c r="A176">
         <v>2313401</v>
       </c>
       <c r="B176" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C176">
         <v>0.657</v>
       </c>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:3">
       <c r="A177">
         <v>2313500</v>
       </c>
       <c r="B177" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C177">
         <v>0.606</v>
       </c>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:3">
       <c r="A178">
         <v>2313559</v>
       </c>
       <c r="B178" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C178">
         <v>0.606</v>
       </c>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:3">
       <c r="A179">
         <v>2313609</v>
       </c>
       <c r="B179" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C179">
         <v>0.648</v>
       </c>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:3">
       <c r="A180">
         <v>2313708</v>
       </c>
       <c r="B180" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C180">
         <v>0.591</v>
       </c>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:3">
       <c r="A181">
         <v>2313757</v>
       </c>
       <c r="B181" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C181">
         <v>0.587</v>
       </c>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:3">
       <c r="A182">
         <v>2313807</v>
       </c>
       <c r="B182" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C182">
         <v>0.639</v>
       </c>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:3">
       <c r="A183">
         <v>2313906</v>
       </c>
       <c r="B183" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C183">
         <v>0.5659999999999999</v>
       </c>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:3">
       <c r="A184">
         <v>2313955</v>
       </c>
       <c r="B184" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C184">
         <v>0.611</v>
       </c>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:3">
       <c r="A185">
         <v>2314003</v>
       </c>
       <c r="B185" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C185">
         <v>0.629</v>
       </c>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:3">
       <c r="A186">
         <v>2314102</v>
       </c>
       <c r="B186" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C186">
         <v>0.571</v>

</xml_diff>